<commit_message>
verander fallback kilometrage bakwagens naar 32848
</commit_message>
<xml_diff>
--- a/data_template_Sloterdijk_Poort_Noord_v2.xlsx
+++ b/data_template_Sloterdijk_Poort_Noord_v2.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\Bedrijven_dashboard_RWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A857C2D-59E8-45B8-995C-0E8D8B1E4C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983EF66-3DD1-48EB-82B5-6A47CE311AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$U$1:$U$194</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -823,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,7 +1113,7 @@
         <v>54505</v>
       </c>
       <c r="U3" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V3" s="5">
         <v>18000</v>
@@ -1205,7 +1208,7 @@
         <v>54505</v>
       </c>
       <c r="U4" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V4" s="5">
         <v>20000</v>
@@ -1496,7 +1499,7 @@
         <v>54505</v>
       </c>
       <c r="U7" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V7" s="5">
         <v>18000</v>
@@ -1591,7 +1594,7 @@
         <v>54505</v>
       </c>
       <c r="U8" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V8" s="5">
         <v>18000</v>
@@ -1686,7 +1689,7 @@
         <v>54505</v>
       </c>
       <c r="U9" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V9" s="5">
         <v>18000</v>
@@ -1781,7 +1784,7 @@
         <v>54505</v>
       </c>
       <c r="U10" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V10" s="5">
         <v>30000</v>
@@ -1876,7 +1879,7 @@
         <v>54505</v>
       </c>
       <c r="U11" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V11" s="5">
         <v>30000</v>
@@ -1971,7 +1974,7 @@
         <v>54505</v>
       </c>
       <c r="U12" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V12" s="5">
         <v>30000</v>
@@ -2066,7 +2069,7 @@
         <v>54505</v>
       </c>
       <c r="U13" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V13" s="5">
         <v>15000</v>
@@ -2161,7 +2164,7 @@
         <v>54505</v>
       </c>
       <c r="U14" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V14" s="5">
         <v>30000</v>
@@ -2253,7 +2256,7 @@
         <v>54505</v>
       </c>
       <c r="U15" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V15" s="5">
         <v>18000</v>
@@ -2348,7 +2351,7 @@
         <v>54505</v>
       </c>
       <c r="U16" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V16" s="5">
         <v>18000</v>
@@ -2443,7 +2446,7 @@
         <v>54505</v>
       </c>
       <c r="U17" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V17" s="5">
         <v>18000</v>
@@ -2538,7 +2541,7 @@
         <v>54505</v>
       </c>
       <c r="U18" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V18" s="5">
         <v>18000</v>
@@ -2633,7 +2636,7 @@
         <v>54505</v>
       </c>
       <c r="U19" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V19" s="5">
         <v>30000</v>
@@ -2728,7 +2731,7 @@
         <v>54505</v>
       </c>
       <c r="U20" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V20" s="5">
         <v>18000</v>
@@ -2823,7 +2826,7 @@
         <v>54505</v>
       </c>
       <c r="U21" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V21" s="5">
         <v>18000</v>
@@ -2918,7 +2921,7 @@
         <v>54505</v>
       </c>
       <c r="U22" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V22" s="5">
         <v>30000</v>
@@ -3108,7 +3111,7 @@
         <v>54505</v>
       </c>
       <c r="U24" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V24" s="5">
         <v>18000</v>
@@ -3203,7 +3206,7 @@
         <v>54505</v>
       </c>
       <c r="U25" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V25" s="5">
         <v>18000</v>
@@ -3298,7 +3301,7 @@
         <v>54505</v>
       </c>
       <c r="U26" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V26" s="5">
         <v>130000</v>
@@ -3393,7 +3396,7 @@
         <v>54505</v>
       </c>
       <c r="U27" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V27" s="5">
         <v>18000</v>
@@ -3488,7 +3491,7 @@
         <v>54505</v>
       </c>
       <c r="U28" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V28" s="5">
         <v>20000</v>
@@ -3583,7 +3586,7 @@
         <v>54505</v>
       </c>
       <c r="U29" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V29" s="5">
         <v>18000</v>
@@ -3678,7 +3681,7 @@
         <v>54505</v>
       </c>
       <c r="U30" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V30" s="5">
         <v>18000</v>
@@ -3773,7 +3776,7 @@
         <v>54505</v>
       </c>
       <c r="U31" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V31" s="5">
         <v>18000</v>
@@ -3868,7 +3871,7 @@
         <v>54505</v>
       </c>
       <c r="U32" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V32" s="5">
         <v>18000</v>
@@ -3963,7 +3966,7 @@
         <v>54505</v>
       </c>
       <c r="U33" s="5">
-        <v>54505</v>
+        <v>32848</v>
       </c>
       <c r="V33" s="5">
         <v>18000</v>
@@ -4563,6 +4566,7 @@
     <row r="193" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="194" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <autoFilter ref="U1:U194" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add sligro panden to profielen
</commit_message>
<xml_diff>
--- a/data_template_Sloterdijk_Poort_Noord_v2.xlsx
+++ b/data_template_Sloterdijk_Poort_Noord_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\Bedrijven_dashboard_RWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6983EF66-3DD1-48EB-82B5-6A47CE311AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB87ED8B-24A8-46BC-B29F-946F4DFB2456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="123">
   <si>
     <t>bedrijfsnaam</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>HULSHOFF SMART</t>
+  </si>
+  <si>
+    <t>SLIGRO_PAND</t>
   </si>
 </sst>
 </file>
@@ -826,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,7 +985,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="K2" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
change name of company
</commit_message>
<xml_diff>
--- a/data_template_Sloterdijk_Poort_Noord_v2.xlsx
+++ b/data_template_Sloterdijk_Poort_Noord_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\Bedrijven_dashboard_RWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB87ED8B-24A8-46BC-B29F-946F4DFB2456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F2BD55-113A-45A8-8AC9-F4DC8EA61123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
     <t>HULSHOFF SMART</t>
   </si>
   <si>
-    <t>SLIGRO_PAND</t>
+    <t>GOUD_PAND</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
   <dimension ref="A1:AF194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>